<commit_message>
Arreglo para poder usar subclases
Se arregla el codigo para poder usar referencias de unas subclases a otras en lugar de poner metodos estaticos. Se cambia el nombre de la clase Math a MyMath para que no entre en conflicto con la libreria del sistema. Se añaden los using necesarios para que funcionen las fuciones de todos los ficheros.
</commit_message>
<xml_diff>
--- a/DIRECTORIO_FUNCIONES.xlsx
+++ b/DIRECTORIO_FUNCIONES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InSync\GitHub\Producto-Desarrollo-Herramientas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6137DFBF-2C38-411C-86CC-7F8DDC07AA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A33F2F-EA27-4BBA-B94F-96D26ED67F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{109BCD2E-DB73-49E5-A85A-7F976E2CCA1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{109BCD2E-DB73-49E5-A85A-7F976E2CCA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="WINDOWS" sheetId="8" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="335">
   <si>
     <t>Nombre</t>
   </si>
@@ -1051,6 +1051,12 @@
   </si>
   <si>
     <t>Dar formato de encabezado de las tablas de reacciones que saca SAP2000 a un excel que queramos en un rango dado. Solo pone el formato, no el texto.</t>
+  </si>
+  <si>
+    <t>UnlockModel</t>
+  </si>
+  <si>
+    <t>Desbloquea un modelo SAP2000 calculado.</t>
   </si>
 </sst>
 </file>
@@ -2229,26 +2235,77 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2259,125 +2316,137 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2394,54 +2463,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2450,21 +2471,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2810,8 +2816,8 @@
   </sheetPr>
   <dimension ref="B1:J170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,29 +2832,29 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -2867,7 +2873,7 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
@@ -2876,13 +2882,13 @@
       <c r="C4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="128" t="s">
+      <c r="E4" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="194" t="s">
+      <c r="F4" s="131" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="30" t="s">
@@ -2908,7 +2914,7 @@
       <c r="D5" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="196" t="s">
+      <c r="E5" s="133" t="s">
         <v>324</v>
       </c>
       <c r="F5" s="110" t="s">
@@ -2934,13 +2940,13 @@
       <c r="C6" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="193" t="s">
+      <c r="E6" s="130" t="s">
         <v>324</v>
       </c>
-      <c r="F6" s="195" t="s">
+      <c r="F6" s="132" t="s">
         <v>325</v>
       </c>
       <c r="G6" s="30" t="s">
@@ -2986,10 +2992,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="136" t="s">
+      <c r="C8" s="141" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="35" t="s">
@@ -3001,22 +3007,22 @@
       <c r="F8" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="138" t="s">
+      <c r="G8" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="140" t="s">
+      <c r="H8" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="142" t="s">
+      <c r="I8" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="136" t="s">
+      <c r="J8" s="141" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="137"/>
-      <c r="C9" s="137"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
       <c r="D9" s="7" t="s">
         <v>64</v>
       </c>
@@ -3026,10 +3032,10 @@
       <c r="F9" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="139"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="143"/>
-      <c r="J9" s="137"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="148"/>
+      <c r="J9" s="142"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
@@ -4833,8 +4839,8 @@
   </sheetPr>
   <dimension ref="B1:J168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4855,29 +4861,29 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -4896,7 +4902,7 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
@@ -4957,10 +4963,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="149" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="35" t="s">
@@ -4972,22 +4978,22 @@
       <c r="F6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="138" t="s">
+      <c r="G6" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="140" t="s">
+      <c r="H6" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="152" t="s">
+      <c r="I6" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="144" t="s">
+      <c r="J6" s="149" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="150"/>
       <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
@@ -4997,10 +5003,10 @@
       <c r="F7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="139"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="145"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="150"/>
     </row>
     <row r="8" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="40" t="s">
@@ -5032,10 +5038,10 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="144" t="s">
+      <c r="C9" s="149" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="35" t="s">
@@ -5047,22 +5053,22 @@
       <c r="F9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="138" t="s">
+      <c r="G9" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="140" t="s">
+      <c r="H9" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="152" t="s">
+      <c r="I9" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="136" t="s">
+      <c r="J9" s="141" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="154"/>
-      <c r="C10" s="154"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="164"/>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
@@ -5072,14 +5078,14 @@
       <c r="F10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="161"/>
-      <c r="H10" s="162"/>
-      <c r="I10" s="163"/>
-      <c r="J10" s="167"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="166"/>
+      <c r="I10" s="167"/>
+      <c r="J10" s="168"/>
     </row>
     <row r="11" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="145"/>
-      <c r="C11" s="145"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
       <c r="D11" s="7" t="s">
         <v>38</v>
       </c>
@@ -5089,16 +5095,16 @@
       <c r="F11" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="139"/>
-      <c r="H11" s="141"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="137"/>
+      <c r="G11" s="144"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="158"/>
+      <c r="J11" s="142"/>
     </row>
     <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="156" t="s">
+      <c r="B12" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="156" t="s">
+      <c r="C12" s="169" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -5110,22 +5116,22 @@
       <c r="F12" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="146" t="s">
+      <c r="G12" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="148" t="s">
+      <c r="H12" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="150" t="s">
+      <c r="I12" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="168" t="s">
+      <c r="J12" s="163" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="156"/>
-      <c r="C13" s="156"/>
+      <c r="B13" s="169"/>
+      <c r="C13" s="169"/>
       <c r="D13" s="48" t="s">
         <v>45</v>
       </c>
@@ -5135,16 +5141,16 @@
       <c r="F13" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="147"/>
-      <c r="H13" s="149"/>
-      <c r="I13" s="151"/>
-      <c r="J13" s="168"/>
+      <c r="G13" s="162"/>
+      <c r="H13" s="152"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="163"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="144" t="s">
+      <c r="C14" s="149" t="s">
         <v>70</v>
       </c>
       <c r="D14" s="35" t="s">
@@ -5156,22 +5162,22 @@
       <c r="F14" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="138" t="s">
+      <c r="G14" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="140" t="s">
+      <c r="H14" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="152" t="s">
+      <c r="I14" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="136" t="s">
+      <c r="J14" s="141" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="150"/>
       <c r="D15" s="7" t="s">
         <v>23</v>
       </c>
@@ -5181,16 +5187,16 @@
       <c r="F15" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="139"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="137"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="158"/>
+      <c r="J15" s="142"/>
     </row>
     <row r="16" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="155" t="s">
+      <c r="C16" s="159" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="61" t="s">
@@ -5202,22 +5208,22 @@
       <c r="F16" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="146" t="s">
+      <c r="G16" s="161" t="s">
         <v>162</v>
       </c>
-      <c r="H16" s="148" t="s">
+      <c r="H16" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="150" t="s">
+      <c r="I16" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="155" t="s">
+      <c r="J16" s="159" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="157"/>
-      <c r="C17" s="157"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="160"/>
       <c r="D17" s="67" t="s">
         <v>7</v>
       </c>
@@ -5227,10 +5233,10 @@
       <c r="F17" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="147"/>
-      <c r="H17" s="149"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="157"/>
+      <c r="G17" s="162"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="160"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="29" t="s">
@@ -5262,10 +5268,10 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="155" t="s">
+      <c r="B19" s="159" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="155" t="s">
+      <c r="C19" s="159" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="61" t="s">
@@ -5277,22 +5283,22 @@
       <c r="F19" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="146" t="s">
+      <c r="G19" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="148" t="s">
+      <c r="H19" s="151" t="s">
         <v>200</v>
       </c>
-      <c r="I19" s="150" t="s">
+      <c r="I19" s="153" t="s">
         <v>201</v>
       </c>
-      <c r="J19" s="155" t="s">
+      <c r="J19" s="159" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
       <c r="D20" s="67" t="s">
         <v>64</v>
       </c>
@@ -5302,16 +5308,16 @@
       <c r="F20" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="G20" s="147"/>
-      <c r="H20" s="149"/>
-      <c r="I20" s="151"/>
-      <c r="J20" s="157"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="160"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="144" t="s">
+      <c r="B21" s="149" t="s">
         <v>211</v>
       </c>
-      <c r="C21" s="144" t="s">
+      <c r="C21" s="149" t="s">
         <v>212</v>
       </c>
       <c r="D21" s="35" t="s">
@@ -5323,22 +5329,22 @@
       <c r="F21" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="138" t="s">
+      <c r="G21" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="140" t="s">
+      <c r="H21" s="145" t="s">
         <v>215</v>
       </c>
-      <c r="I21" s="152" t="s">
+      <c r="I21" s="157" t="s">
         <v>216</v>
       </c>
-      <c r="J21" s="136" t="s">
+      <c r="J21" s="141" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="166"/>
-      <c r="C22" s="145"/>
+      <c r="B22" s="173"/>
+      <c r="C22" s="150"/>
       <c r="D22" s="7" t="s">
         <v>45</v>
       </c>
@@ -5348,16 +5354,16 @@
       <c r="F22" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="G22" s="139"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="153"/>
-      <c r="J22" s="137"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="142"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="159" t="s">
         <v>218</v>
       </c>
-      <c r="C23" s="155" t="s">
+      <c r="C23" s="159" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="61" t="s">
@@ -5369,22 +5375,22 @@
       <c r="F23" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="146" t="s">
+      <c r="G23" s="161" t="s">
         <v>221</v>
       </c>
-      <c r="H23" s="148" t="s">
+      <c r="H23" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="I23" s="150" t="s">
+      <c r="I23" s="153" t="s">
         <v>223</v>
       </c>
-      <c r="J23" s="164" t="s">
+      <c r="J23" s="155" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="160"/>
       <c r="D24" s="67" t="s">
         <v>7</v>
       </c>
@@ -5394,16 +5400,16 @@
       <c r="F24" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="G24" s="147"/>
-      <c r="H24" s="149"/>
-      <c r="I24" s="151"/>
-      <c r="J24" s="165"/>
+      <c r="G24" s="162"/>
+      <c r="H24" s="152"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="144" t="s">
+      <c r="B25" s="149" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="149" t="s">
         <v>71</v>
       </c>
       <c r="D25" s="35" t="s">
@@ -5415,22 +5421,22 @@
       <c r="F25" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="138" t="s">
+      <c r="G25" s="143" t="s">
         <v>221</v>
       </c>
-      <c r="H25" s="140" t="s">
+      <c r="H25" s="145" t="s">
         <v>233</v>
       </c>
-      <c r="I25" s="152" t="s">
+      <c r="I25" s="157" t="s">
         <v>234</v>
       </c>
-      <c r="J25" s="136" t="s">
+      <c r="J25" s="141" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="154"/>
-      <c r="C26" s="154"/>
+      <c r="B26" s="164"/>
+      <c r="C26" s="164"/>
       <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
@@ -5440,14 +5446,14 @@
       <c r="F26" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="G26" s="161"/>
-      <c r="H26" s="162"/>
-      <c r="I26" s="163"/>
-      <c r="J26" s="154"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="167"/>
+      <c r="J26" s="164"/>
     </row>
     <row r="27" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="154"/>
-      <c r="C27" s="154"/>
+      <c r="B27" s="164"/>
+      <c r="C27" s="164"/>
       <c r="D27" s="3" t="s">
         <v>45</v>
       </c>
@@ -5457,14 +5463,14 @@
       <c r="F27" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="161"/>
-      <c r="H27" s="162"/>
-      <c r="I27" s="163"/>
-      <c r="J27" s="154"/>
+      <c r="G27" s="165"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="167"/>
+      <c r="J27" s="164"/>
     </row>
     <row r="28" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
       <c r="D28" s="7" t="s">
         <v>230</v>
       </c>
@@ -5474,16 +5480,16 @@
       <c r="F28" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="G28" s="139"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="153"/>
-      <c r="J28" s="145"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="150"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="155" t="s">
+      <c r="B29" s="159" t="s">
         <v>236</v>
       </c>
-      <c r="C29" s="155" t="s">
+      <c r="C29" s="159" t="s">
         <v>212</v>
       </c>
       <c r="D29" s="61" t="s">
@@ -5495,22 +5501,22 @@
       <c r="F29" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="146" t="s">
+      <c r="G29" s="161" t="s">
         <v>221</v>
       </c>
-      <c r="H29" s="148" t="s">
+      <c r="H29" s="151" t="s">
         <v>240</v>
       </c>
-      <c r="I29" s="150" t="s">
+      <c r="I29" s="153" t="s">
         <v>241</v>
       </c>
-      <c r="J29" s="155" t="s">
+      <c r="J29" s="159" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="156"/>
-      <c r="C30" s="156"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="169"/>
       <c r="D30" s="64" t="s">
         <v>182</v>
       </c>
@@ -5520,14 +5526,14 @@
       <c r="F30" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="G30" s="158"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="160"/>
-      <c r="J30" s="156"/>
+      <c r="G30" s="170"/>
+      <c r="H30" s="171"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="169"/>
     </row>
     <row r="31" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="157"/>
-      <c r="C31" s="157"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="160"/>
       <c r="D31" s="67" t="s">
         <v>230</v>
       </c>
@@ -5537,16 +5543,16 @@
       <c r="F31" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="G31" s="147"/>
-      <c r="H31" s="149"/>
-      <c r="I31" s="151"/>
-      <c r="J31" s="157"/>
+      <c r="G31" s="162"/>
+      <c r="H31" s="152"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="160"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="149" t="s">
         <v>243</v>
       </c>
-      <c r="C32" s="144" t="s">
+      <c r="C32" s="149" t="s">
         <v>212</v>
       </c>
       <c r="D32" s="35" t="s">
@@ -5558,22 +5564,22 @@
       <c r="F32" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="138" t="s">
+      <c r="G32" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="H32" s="140" t="s">
+      <c r="H32" s="145" t="s">
         <v>245</v>
       </c>
-      <c r="I32" s="152" t="s">
+      <c r="I32" s="157" t="s">
         <v>246</v>
       </c>
-      <c r="J32" s="144" t="s">
+      <c r="J32" s="149" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="145"/>
-      <c r="C33" s="145"/>
+      <c r="B33" s="150"/>
+      <c r="C33" s="150"/>
       <c r="D33" s="7" t="s">
         <v>230</v>
       </c>
@@ -5583,16 +5589,16 @@
       <c r="F33" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="G33" s="139"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="153"/>
-      <c r="J33" s="145"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="146"/>
+      <c r="I33" s="158"/>
+      <c r="J33" s="150"/>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="155" t="s">
+      <c r="B34" s="159" t="s">
         <v>248</v>
       </c>
-      <c r="C34" s="155" t="s">
+      <c r="C34" s="159" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="61" t="s">
@@ -5604,22 +5610,22 @@
       <c r="F34" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="146" t="s">
+      <c r="G34" s="161" t="s">
         <v>221</v>
       </c>
-      <c r="H34" s="148" t="s">
+      <c r="H34" s="151" t="s">
         <v>233</v>
       </c>
-      <c r="I34" s="150" t="s">
+      <c r="I34" s="153" t="s">
         <v>251</v>
       </c>
-      <c r="J34" s="164" t="s">
+      <c r="J34" s="155" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="156"/>
-      <c r="C35" s="156"/>
+      <c r="B35" s="169"/>
+      <c r="C35" s="169"/>
       <c r="D35" s="117" t="s">
         <v>7</v>
       </c>
@@ -5629,14 +5635,14 @@
       <c r="F35" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="G35" s="158"/>
-      <c r="H35" s="159"/>
-      <c r="I35" s="160"/>
-      <c r="J35" s="168"/>
+      <c r="G35" s="170"/>
+      <c r="H35" s="171"/>
+      <c r="I35" s="172"/>
+      <c r="J35" s="163"/>
     </row>
     <row r="36" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="157"/>
-      <c r="C36" s="157"/>
+      <c r="B36" s="160"/>
+      <c r="C36" s="160"/>
       <c r="D36" s="67" t="s">
         <v>7</v>
       </c>
@@ -5646,16 +5652,16 @@
       <c r="F36" s="69" t="s">
         <v>250</v>
       </c>
-      <c r="G36" s="147"/>
-      <c r="H36" s="149"/>
-      <c r="I36" s="151"/>
-      <c r="J36" s="165"/>
+      <c r="G36" s="162"/>
+      <c r="H36" s="152"/>
+      <c r="I36" s="154"/>
+      <c r="J36" s="156"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="144" t="s">
+      <c r="B37" s="149" t="s">
         <v>253</v>
       </c>
-      <c r="C37" s="144" t="s">
+      <c r="C37" s="149" t="s">
         <v>212</v>
       </c>
       <c r="D37" s="35" t="s">
@@ -5667,22 +5673,22 @@
       <c r="F37" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="138" t="s">
+      <c r="G37" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="H37" s="140" t="s">
+      <c r="H37" s="145" t="s">
         <v>258</v>
       </c>
-      <c r="I37" s="152" t="s">
+      <c r="I37" s="157" t="s">
         <v>259</v>
       </c>
-      <c r="J37" s="136" t="s">
+      <c r="J37" s="141" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="154"/>
-      <c r="C38" s="154"/>
+      <c r="B38" s="164"/>
+      <c r="C38" s="164"/>
       <c r="D38" s="3" t="s">
         <v>182</v>
       </c>
@@ -5692,14 +5698,14 @@
       <c r="F38" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="G38" s="161"/>
-      <c r="H38" s="162"/>
-      <c r="I38" s="163"/>
-      <c r="J38" s="167"/>
+      <c r="G38" s="165"/>
+      <c r="H38" s="166"/>
+      <c r="I38" s="167"/>
+      <c r="J38" s="168"/>
     </row>
     <row r="39" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="145"/>
-      <c r="C39" s="145"/>
+      <c r="B39" s="150"/>
+      <c r="C39" s="150"/>
       <c r="D39" s="7" t="s">
         <v>45</v>
       </c>
@@ -5709,10 +5715,10 @@
       <c r="F39" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="G39" s="139"/>
-      <c r="H39" s="141"/>
-      <c r="I39" s="153"/>
-      <c r="J39" s="137"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="146"/>
+      <c r="I39" s="158"/>
+      <c r="J39" s="142"/>
     </row>
     <row r="40" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="75" t="s">
@@ -5918,39 +5924,39 @@
       </c>
     </row>
     <row r="47" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="120" t="s">
+      <c r="B47" s="119" t="s">
         <v>286</v>
       </c>
-      <c r="C47" s="120" t="s">
+      <c r="C47" s="119" t="s">
         <v>262</v>
       </c>
-      <c r="D47" s="121" t="s">
+      <c r="D47" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="122" t="s">
+      <c r="E47" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="123" t="s">
+      <c r="F47" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="G47" s="121" t="s">
+      <c r="G47" s="120" t="s">
         <v>270</v>
       </c>
-      <c r="H47" s="122" t="s">
+      <c r="H47" s="121" t="s">
         <v>288</v>
       </c>
-      <c r="I47" s="124" t="s">
+      <c r="I47" s="123" t="s">
         <v>290</v>
       </c>
-      <c r="J47" s="125" t="s">
+      <c r="J47" s="124" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="155" t="s">
+      <c r="B48" s="159" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="155" t="s">
+      <c r="C48" s="159" t="s">
         <v>262</v>
       </c>
       <c r="D48" s="61" t="s">
@@ -5962,22 +5968,22 @@
       <c r="F48" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G48" s="146" t="s">
+      <c r="G48" s="161" t="s">
         <v>64</v>
       </c>
-      <c r="H48" s="148" t="s">
+      <c r="H48" s="151" t="s">
         <v>293</v>
       </c>
-      <c r="I48" s="150" t="s">
+      <c r="I48" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="J48" s="164" t="s">
+      <c r="J48" s="155" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="157"/>
-      <c r="C49" s="157"/>
+      <c r="B49" s="160"/>
+      <c r="C49" s="160"/>
       <c r="D49" s="67" t="s">
         <v>38</v>
       </c>
@@ -5987,16 +5993,16 @@
       <c r="F49" s="69" t="s">
         <v>300</v>
       </c>
-      <c r="G49" s="147"/>
-      <c r="H49" s="149"/>
-      <c r="I49" s="151"/>
-      <c r="J49" s="165"/>
+      <c r="G49" s="162"/>
+      <c r="H49" s="152"/>
+      <c r="I49" s="154"/>
+      <c r="J49" s="156"/>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="144" t="s">
+      <c r="B50" s="149" t="s">
         <v>301</v>
       </c>
-      <c r="C50" s="144" t="s">
+      <c r="C50" s="149" t="s">
         <v>262</v>
       </c>
       <c r="D50" s="35" t="s">
@@ -6008,22 +6014,22 @@
       <c r="F50" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G50" s="138" t="s">
+      <c r="G50" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="H50" s="140" t="s">
+      <c r="H50" s="145" t="s">
         <v>304</v>
       </c>
-      <c r="I50" s="152" t="s">
+      <c r="I50" s="157" t="s">
         <v>305</v>
       </c>
-      <c r="J50" s="136" t="s">
+      <c r="J50" s="141" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="145"/>
-      <c r="C51" s="145"/>
+      <c r="B51" s="150"/>
+      <c r="C51" s="150"/>
       <c r="D51" s="7" t="s">
         <v>38</v>
       </c>
@@ -6033,16 +6039,16 @@
       <c r="F51" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="G51" s="139"/>
-      <c r="H51" s="141"/>
-      <c r="I51" s="153"/>
-      <c r="J51" s="137"/>
+      <c r="G51" s="144"/>
+      <c r="H51" s="146"/>
+      <c r="I51" s="158"/>
+      <c r="J51" s="142"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="155" t="s">
+      <c r="B52" s="159" t="s">
         <v>307</v>
       </c>
-      <c r="C52" s="155" t="s">
+      <c r="C52" s="159" t="s">
         <v>262</v>
       </c>
       <c r="D52" s="61" t="s">
@@ -6054,22 +6060,22 @@
       <c r="F52" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G52" s="146" t="s">
+      <c r="G52" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="148" t="s">
+      <c r="H52" s="151" t="s">
         <v>308</v>
       </c>
-      <c r="I52" s="150" t="s">
+      <c r="I52" s="153" t="s">
         <v>309</v>
       </c>
-      <c r="J52" s="164" t="s">
+      <c r="J52" s="155" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="157"/>
-      <c r="C53" s="157"/>
+      <c r="B53" s="160"/>
+      <c r="C53" s="160"/>
       <c r="D53" s="67" t="s">
         <v>38</v>
       </c>
@@ -6079,16 +6085,16 @@
       <c r="F53" s="69" t="s">
         <v>303</v>
       </c>
-      <c r="G53" s="147"/>
-      <c r="H53" s="149"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="165"/>
+      <c r="G53" s="162"/>
+      <c r="H53" s="152"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="156"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="144" t="s">
+      <c r="B54" s="149" t="s">
         <v>311</v>
       </c>
-      <c r="C54" s="144" t="s">
+      <c r="C54" s="149" t="s">
         <v>262</v>
       </c>
       <c r="D54" s="35" t="s">
@@ -6100,22 +6106,22 @@
       <c r="F54" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="138" t="s">
+      <c r="G54" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="H54" s="140" t="s">
+      <c r="H54" s="145" t="s">
         <v>312</v>
       </c>
-      <c r="I54" s="152" t="s">
+      <c r="I54" s="157" t="s">
         <v>313</v>
       </c>
-      <c r="J54" s="136" t="s">
+      <c r="J54" s="141" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="145"/>
-      <c r="C55" s="145"/>
+      <c r="B55" s="150"/>
+      <c r="C55" s="150"/>
       <c r="D55" s="7" t="s">
         <v>38</v>
       </c>
@@ -6125,16 +6131,16 @@
       <c r="F55" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="G55" s="139"/>
-      <c r="H55" s="141"/>
-      <c r="I55" s="153"/>
-      <c r="J55" s="137"/>
+      <c r="G55" s="144"/>
+      <c r="H55" s="146"/>
+      <c r="I55" s="158"/>
+      <c r="J55" s="142"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="155" t="s">
+      <c r="B56" s="159" t="s">
         <v>315</v>
       </c>
-      <c r="C56" s="155" t="s">
+      <c r="C56" s="159" t="s">
         <v>262</v>
       </c>
       <c r="D56" s="61" t="s">
@@ -6146,22 +6152,22 @@
       <c r="F56" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G56" s="146" t="s">
+      <c r="G56" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="H56" s="148" t="s">
+      <c r="H56" s="151" t="s">
         <v>316</v>
       </c>
-      <c r="I56" s="150" t="s">
+      <c r="I56" s="153" t="s">
         <v>317</v>
       </c>
-      <c r="J56" s="164" t="s">
+      <c r="J56" s="155" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="157"/>
-      <c r="C57" s="157"/>
+      <c r="B57" s="160"/>
+      <c r="C57" s="160"/>
       <c r="D57" s="67" t="s">
         <v>38</v>
       </c>
@@ -6171,16 +6177,16 @@
       <c r="F57" s="69" t="s">
         <v>303</v>
       </c>
-      <c r="G57" s="147"/>
-      <c r="H57" s="149"/>
-      <c r="I57" s="151"/>
-      <c r="J57" s="165"/>
+      <c r="G57" s="162"/>
+      <c r="H57" s="152"/>
+      <c r="I57" s="154"/>
+      <c r="J57" s="156"/>
     </row>
     <row r="58" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="144" t="s">
+      <c r="B58" s="149" t="s">
         <v>319</v>
       </c>
-      <c r="C58" s="144" t="s">
+      <c r="C58" s="149" t="s">
         <v>262</v>
       </c>
       <c r="D58" s="35" t="s">
@@ -6192,22 +6198,22 @@
       <c r="F58" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G58" s="138" t="s">
+      <c r="G58" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="140" t="s">
+      <c r="H58" s="145" t="s">
         <v>320</v>
       </c>
-      <c r="I58" s="152" t="s">
+      <c r="I58" s="157" t="s">
         <v>321</v>
       </c>
-      <c r="J58" s="144" t="s">
+      <c r="J58" s="149" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="145"/>
-      <c r="C59" s="145"/>
+      <c r="B59" s="150"/>
+      <c r="C59" s="150"/>
       <c r="D59" s="7" t="s">
         <v>64</v>
       </c>
@@ -6217,32 +6223,50 @@
       <c r="F59" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="G59" s="139"/>
-      <c r="H59" s="141"/>
-      <c r="I59" s="153"/>
-      <c r="J59" s="145"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="108"/>
-      <c r="J60" s="119"/>
+      <c r="G59" s="144"/>
+      <c r="H59" s="146"/>
+      <c r="I59" s="158"/>
+      <c r="J59" s="150"/>
+    </row>
+    <row r="60" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="75" t="s">
+        <v>333</v>
+      </c>
+      <c r="C60" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="110" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" s="80" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="107"/>
-      <c r="J61" s="5"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="108"/>
+      <c r="J61" s="129"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
@@ -7429,63 +7453,44 @@
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="119">
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J25:J28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="J23:J24"/>
@@ -7510,44 +7515,63 @@
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="I9:I11"/>
     <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="H25:H28"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J25:J28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="H58:H59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7560,7 +7584,7 @@
   </sheetPr>
   <dimension ref="B1:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
@@ -7580,29 +7604,29 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -7621,13 +7645,13 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="149" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="149" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="35" t="s">
@@ -7639,22 +7663,22 @@
       <c r="F4" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="138" t="s">
+      <c r="G4" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="140" t="s">
+      <c r="H4" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="142" t="s">
+      <c r="I4" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="144" t="s">
+      <c r="J4" s="149" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -7664,14 +7688,14 @@
       <c r="F5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="161"/>
-      <c r="H5" s="162"/>
-      <c r="I5" s="189"/>
-      <c r="J5" s="154"/>
+      <c r="G5" s="165"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="164"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="154"/>
-      <c r="C6" s="154"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="164"/>
       <c r="D6" s="3" t="s">
         <v>81</v>
       </c>
@@ -7681,14 +7705,14 @@
       <c r="F6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="161"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="189"/>
-      <c r="J6" s="154"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="166"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="164"/>
     </row>
     <row r="7" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="154"/>
-      <c r="C7" s="154"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
       <c r="D7" s="3" t="s">
         <v>82</v>
       </c>
@@ -7698,14 +7722,14 @@
       <c r="F7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="161"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="189"/>
-      <c r="J7" s="154"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="166"/>
+      <c r="I7" s="174"/>
+      <c r="J7" s="164"/>
     </row>
     <row r="8" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="150"/>
       <c r="D8" s="7" t="s">
         <v>82</v>
       </c>
@@ -7715,16 +7739,16 @@
       <c r="F8" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="141"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="145"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="150"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="159" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="155" t="s">
+      <c r="C9" s="159" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="61" t="s">
@@ -7736,22 +7760,22 @@
       <c r="F9" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="146" t="s">
+      <c r="G9" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="148" t="s">
+      <c r="H9" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="174" t="s">
+      <c r="I9" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="155" t="s">
+      <c r="J9" s="159" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="156"/>
-      <c r="C10" s="156"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="169"/>
       <c r="D10" s="64" t="s">
         <v>94</v>
       </c>
@@ -7761,14 +7785,14 @@
       <c r="F10" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="158"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="188"/>
-      <c r="J10" s="156"/>
+      <c r="G10" s="170"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="176"/>
+      <c r="J10" s="169"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
       <c r="D11" s="67" t="s">
         <v>81</v>
       </c>
@@ -7778,16 +7802,16 @@
       <c r="F11" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="147"/>
-      <c r="H11" s="149"/>
-      <c r="I11" s="175"/>
-      <c r="J11" s="157"/>
+      <c r="G11" s="162"/>
+      <c r="H11" s="152"/>
+      <c r="I11" s="177"/>
+      <c r="J11" s="160"/>
     </row>
     <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="149" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="144" t="s">
+      <c r="C12" s="149" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="35" t="s">
@@ -7799,22 +7823,22 @@
       <c r="F12" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="138" t="s">
+      <c r="G12" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="140" t="s">
+      <c r="H12" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="142" t="s">
+      <c r="I12" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="144" t="s">
+      <c r="J12" s="149" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="154"/>
-      <c r="C13" s="154"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="164"/>
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
@@ -7824,14 +7848,14 @@
       <c r="F13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="161"/>
-      <c r="H13" s="162"/>
-      <c r="I13" s="189"/>
-      <c r="J13" s="154"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="164"/>
     </row>
     <row r="14" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="154"/>
-      <c r="C14" s="154"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="164"/>
       <c r="D14" s="3" t="s">
         <v>64</v>
       </c>
@@ -7841,14 +7865,14 @@
       <c r="F14" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="161"/>
-      <c r="H14" s="162"/>
-      <c r="I14" s="189"/>
-      <c r="J14" s="154"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="174"/>
+      <c r="J14" s="164"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="164"/>
       <c r="D15" s="3" t="s">
         <v>81</v>
       </c>
@@ -7858,14 +7882,14 @@
       <c r="F15" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="161"/>
-      <c r="H15" s="162"/>
-      <c r="I15" s="189"/>
-      <c r="J15" s="154"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="174"/>
+      <c r="J15" s="164"/>
     </row>
     <row r="16" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="164"/>
       <c r="D16" s="3" t="s">
         <v>82</v>
       </c>
@@ -7875,14 +7899,14 @@
       <c r="F16" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="161"/>
-      <c r="H16" s="162"/>
-      <c r="I16" s="189"/>
-      <c r="J16" s="154"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="174"/>
+      <c r="J16" s="164"/>
     </row>
     <row r="17" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="145"/>
-      <c r="C17" s="145"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150"/>
       <c r="D17" s="7" t="s">
         <v>82</v>
       </c>
@@ -7892,16 +7916,16 @@
       <c r="F17" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="139"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="143"/>
-      <c r="J17" s="145"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="148"/>
+      <c r="J17" s="150"/>
     </row>
     <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="155" t="s">
+      <c r="C18" s="159" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="61" t="s">
@@ -7913,22 +7937,22 @@
       <c r="F18" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="146" t="s">
+      <c r="G18" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="148" t="s">
+      <c r="H18" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="174" t="s">
+      <c r="I18" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="155" t="s">
+      <c r="J18" s="159" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="156"/>
-      <c r="C19" s="156"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="169"/>
       <c r="D19" s="64" t="s">
         <v>94</v>
       </c>
@@ -7938,14 +7962,14 @@
       <c r="F19" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="158"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="188"/>
-      <c r="J19" s="156"/>
+      <c r="G19" s="170"/>
+      <c r="H19" s="171"/>
+      <c r="I19" s="176"/>
+      <c r="J19" s="169"/>
     </row>
     <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="156"/>
-      <c r="C20" s="156"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
       <c r="D20" s="64" t="s">
         <v>94</v>
       </c>
@@ -7955,14 +7979,14 @@
       <c r="F20" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="159"/>
-      <c r="I20" s="188"/>
-      <c r="J20" s="156"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="171"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="169"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="160"/>
       <c r="D21" s="67" t="s">
         <v>81</v>
       </c>
@@ -7972,10 +7996,10 @@
       <c r="F21" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="G21" s="147"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="175"/>
-      <c r="J21" s="157"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="177"/>
+      <c r="J21" s="160"/>
     </row>
     <row r="22" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="72" t="s">
@@ -8094,10 +8118,10 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="149" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="149" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="35" t="s">
@@ -8109,22 +8133,22 @@
       <c r="F26" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="138" t="s">
+      <c r="G26" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="140" t="s">
+      <c r="H26" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="142" t="s">
+      <c r="I26" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="144" t="s">
+      <c r="J26" s="149" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="145"/>
-      <c r="C27" s="145"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="150"/>
       <c r="D27" s="58" t="s">
         <v>81</v>
       </c>
@@ -8134,16 +8158,16 @@
       <c r="F27" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="139"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="143"/>
-      <c r="J27" s="145"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="146"/>
+      <c r="I27" s="148"/>
+      <c r="J27" s="150"/>
     </row>
     <row r="28" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="155" t="s">
+      <c r="B28" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="172" t="s">
+      <c r="C28" s="193" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="61" t="s">
@@ -8155,22 +8179,22 @@
       <c r="F28" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="146" t="s">
+      <c r="G28" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="148" t="s">
+      <c r="H28" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="174" t="s">
+      <c r="I28" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="155" t="s">
+      <c r="J28" s="159" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="157"/>
-      <c r="C29" s="173"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="194"/>
       <c r="D29" s="67" t="s">
         <v>81</v>
       </c>
@@ -8180,16 +8204,16 @@
       <c r="F29" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="G29" s="147"/>
-      <c r="H29" s="149"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="157"/>
+      <c r="G29" s="162"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="177"/>
+      <c r="J29" s="160"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="176" t="s">
+      <c r="B30" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="176" t="s">
+      <c r="C30" s="178" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="98" t="s">
@@ -8201,22 +8225,22 @@
       <c r="F30" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="G30" s="179" t="s">
+      <c r="G30" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="182" t="s">
+      <c r="H30" s="184" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="185" t="s">
+      <c r="I30" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="169" t="s">
+      <c r="J30" s="190" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="177"/>
-      <c r="C31" s="177"/>
+      <c r="B31" s="179"/>
+      <c r="C31" s="179"/>
       <c r="D31" s="90" t="s">
         <v>7</v>
       </c>
@@ -8226,14 +8250,14 @@
       <c r="F31" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="G31" s="180"/>
-      <c r="H31" s="183"/>
-      <c r="I31" s="186"/>
-      <c r="J31" s="170"/>
+      <c r="G31" s="182"/>
+      <c r="H31" s="185"/>
+      <c r="I31" s="188"/>
+      <c r="J31" s="191"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="178"/>
-      <c r="C32" s="178"/>
+      <c r="B32" s="180"/>
+      <c r="C32" s="180"/>
       <c r="D32" s="93" t="s">
         <v>81</v>
       </c>
@@ -8243,16 +8267,16 @@
       <c r="F32" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="G32" s="181"/>
-      <c r="H32" s="184"/>
-      <c r="I32" s="187"/>
-      <c r="J32" s="171"/>
+      <c r="G32" s="183"/>
+      <c r="H32" s="186"/>
+      <c r="I32" s="189"/>
+      <c r="J32" s="192"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="155" t="s">
+      <c r="B33" s="159" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="155" t="s">
+      <c r="C33" s="159" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="61" t="s">
@@ -8264,22 +8288,22 @@
       <c r="F33" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="146" t="s">
+      <c r="G33" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="148" t="s">
+      <c r="H33" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I33" s="174" t="s">
+      <c r="I33" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="J33" s="164" t="s">
+      <c r="J33" s="155" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="156"/>
-      <c r="C34" s="156"/>
+      <c r="B34" s="169"/>
+      <c r="C34" s="169"/>
       <c r="D34" s="64" t="s">
         <v>7</v>
       </c>
@@ -8289,14 +8313,14 @@
       <c r="F34" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="G34" s="158"/>
-      <c r="H34" s="159"/>
-      <c r="I34" s="188"/>
-      <c r="J34" s="168"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="171"/>
+      <c r="I34" s="176"/>
+      <c r="J34" s="163"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="160"/>
       <c r="D35" s="67" t="s">
         <v>81</v>
       </c>
@@ -8306,16 +8330,16 @@
       <c r="F35" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="147"/>
-      <c r="H35" s="149"/>
-      <c r="I35" s="175"/>
-      <c r="J35" s="165"/>
+      <c r="G35" s="162"/>
+      <c r="H35" s="152"/>
+      <c r="I35" s="177"/>
+      <c r="J35" s="156"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="176" t="s">
+      <c r="B36" s="178" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="176" t="s">
+      <c r="C36" s="178" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="87" t="s">
@@ -8327,22 +8351,22 @@
       <c r="F36" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="G36" s="179" t="s">
+      <c r="G36" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="182" t="s">
+      <c r="H36" s="184" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="185" t="s">
+      <c r="I36" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="J36" s="169" t="s">
+      <c r="J36" s="190" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="177"/>
-      <c r="C37" s="177"/>
+      <c r="B37" s="179"/>
+      <c r="C37" s="179"/>
       <c r="D37" s="90" t="s">
         <v>7</v>
       </c>
@@ -8352,14 +8376,14 @@
       <c r="F37" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="G37" s="180"/>
-      <c r="H37" s="183"/>
-      <c r="I37" s="186"/>
-      <c r="J37" s="170"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="185"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="191"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="177"/>
-      <c r="C38" s="177"/>
+      <c r="B38" s="179"/>
+      <c r="C38" s="179"/>
       <c r="D38" s="101" t="s">
         <v>81</v>
       </c>
@@ -8369,14 +8393,14 @@
       <c r="F38" s="103" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="180"/>
-      <c r="H38" s="183"/>
-      <c r="I38" s="186"/>
-      <c r="J38" s="170"/>
+      <c r="G38" s="182"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="188"/>
+      <c r="J38" s="191"/>
     </row>
     <row r="39" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="178"/>
-      <c r="C39" s="178"/>
+      <c r="B39" s="180"/>
+      <c r="C39" s="180"/>
       <c r="D39" s="93" t="s">
         <v>82</v>
       </c>
@@ -8386,10 +8410,10 @@
       <c r="F39" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="G39" s="181"/>
-      <c r="H39" s="184"/>
-      <c r="I39" s="187"/>
-      <c r="J39" s="171"/>
+      <c r="G39" s="183"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="189"/>
+      <c r="J39" s="192"/>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="75" t="s">
@@ -8479,10 +8503,10 @@
       </c>
     </row>
     <row r="43" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="144" t="s">
+      <c r="B43" s="149" t="s">
         <v>326</v>
       </c>
-      <c r="C43" s="144" t="s">
+      <c r="C43" s="149" t="s">
         <v>80</v>
       </c>
       <c r="D43" s="35" t="s">
@@ -8500,16 +8524,16 @@
       <c r="H43" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="197" t="s">
+      <c r="I43" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="J43" s="136" t="s">
+      <c r="J43" s="141" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="154"/>
-      <c r="C44" s="154"/>
+      <c r="B44" s="164"/>
+      <c r="C44" s="164"/>
       <c r="D44" s="11" t="s">
         <v>7</v>
       </c>
@@ -8528,12 +8552,12 @@
       <c r="I44" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J44" s="167"/>
+      <c r="J44" s="168"/>
     </row>
     <row r="45" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="145"/>
-      <c r="C45" s="145"/>
-      <c r="D45" s="127" t="s">
+      <c r="B45" s="150"/>
+      <c r="C45" s="150"/>
+      <c r="D45" s="126" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="8" t="s">
@@ -8551,7 +8575,7 @@
       <c r="I45" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J45" s="137"/>
+      <c r="J45" s="142"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
@@ -8562,7 +8586,7 @@
       <c r="G46" s="11"/>
       <c r="H46" s="12"/>
       <c r="I46" s="24"/>
-      <c r="J46" s="129"/>
+      <c r="J46" s="128"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
@@ -9936,6 +9960,52 @@
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="62">
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="J33:J35"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="H12:H17"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="J12:J17"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="J43:J45"/>
@@ -9952,52 +10022,6 @@
     <mergeCell ref="I4:I8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="H12:H17"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="J33:J35"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="G33:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -10033,29 +10057,29 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -10074,13 +10098,13 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="149" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="149" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="35" t="s">
@@ -10101,13 +10125,13 @@
       <c r="I4" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="J4" s="136" t="s">
+      <c r="J4" s="141" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -10126,11 +10150,11 @@
       <c r="I5" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="167"/>
+      <c r="J5" s="168"/>
     </row>
     <row r="6" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
+      <c r="B6" s="150"/>
+      <c r="C6" s="150"/>
       <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
@@ -10149,7 +10173,7 @@
       <c r="I6" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="137"/>
+      <c r="J6" s="142"/>
     </row>
     <row r="7" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="75" t="s">
@@ -10268,10 +10292,10 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="155" t="s">
+      <c r="B11" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="155" t="s">
+      <c r="C11" s="159" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="61" t="s">
@@ -10283,22 +10307,22 @@
       <c r="F11" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="G11" s="146" t="s">
+      <c r="G11" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="148" t="s">
+      <c r="H11" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="150" t="s">
+      <c r="I11" s="153" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="155" t="s">
+      <c r="J11" s="159" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="157"/>
-      <c r="C12" s="157"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
       <c r="D12" s="112" t="s">
         <v>149</v>
       </c>
@@ -10308,10 +10332,10 @@
       <c r="F12" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="G12" s="147"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="157"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="152"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="160"/>
     </row>
     <row r="13" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="29" t="s">
@@ -10372,10 +10396,10 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="149" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="144" t="s">
+      <c r="C15" s="149" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="113" t="s">
@@ -10387,22 +10411,22 @@
       <c r="F15" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="G15" s="138" t="s">
+      <c r="G15" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="140" t="s">
+      <c r="H15" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="152" t="s">
+      <c r="I15" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="136" t="s">
+      <c r="J15" s="141" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="150"/>
       <c r="D16" s="7" t="s">
         <v>64</v>
       </c>
@@ -10412,10 +10436,10 @@
       <c r="F16" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="G16" s="139"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="137"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="146"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="142"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
@@ -12098,11 +12122,12 @@
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="J4:J6"/>
@@ -12112,12 +12137,11 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12144,29 +12168,29 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -12185,7 +12209,7 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
@@ -14015,29 +14039,29 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -14056,13 +14080,13 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="149" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="149" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="35" t="s">
@@ -14074,22 +14098,22 @@
       <c r="F4" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="G4" s="138" t="s">
+      <c r="G4" s="143" t="s">
         <v>162</v>
       </c>
-      <c r="H4" s="140" t="s">
+      <c r="H4" s="145" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="152" t="s">
+      <c r="I4" s="157" t="s">
         <v>181</v>
       </c>
-      <c r="J4" s="136" t="s">
+      <c r="J4" s="141" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="150"/>
       <c r="D5" s="7" t="s">
         <v>176</v>
       </c>
@@ -14099,16 +14123,16 @@
       <c r="F5" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="139"/>
-      <c r="H5" s="141"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="137"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="158"/>
+      <c r="J5" s="142"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="155" t="s">
+      <c r="B6" s="159" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="159" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="61" t="s">
@@ -14120,22 +14144,22 @@
       <c r="F6" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="G6" s="146" t="s">
+      <c r="G6" s="161" t="s">
         <v>162</v>
       </c>
-      <c r="H6" s="148" t="s">
+      <c r="H6" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="150" t="s">
+      <c r="I6" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="J6" s="164" t="s">
+      <c r="J6" s="155" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="156"/>
-      <c r="C7" s="156"/>
+      <c r="B7" s="169"/>
+      <c r="C7" s="169"/>
       <c r="D7" s="64" t="s">
         <v>182</v>
       </c>
@@ -14145,14 +14169,14 @@
       <c r="F7" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="158"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="168"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="163"/>
     </row>
     <row r="8" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="157"/>
-      <c r="C8" s="157"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="160"/>
       <c r="D8" s="67" t="s">
         <v>7</v>
       </c>
@@ -14162,16 +14186,16 @@
       <c r="F8" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="G8" s="147"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="165"/>
+      <c r="G8" s="162"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="156"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="176" t="s">
+      <c r="B9" s="178" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="176" t="s">
+      <c r="C9" s="178" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="87" t="s">
@@ -14183,22 +14207,22 @@
       <c r="F9" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="G9" s="179" t="s">
+      <c r="G9" s="181" t="s">
         <v>162</v>
       </c>
-      <c r="H9" s="182" t="s">
+      <c r="H9" s="184" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="190" t="s">
+      <c r="I9" s="195" t="s">
         <v>187</v>
       </c>
-      <c r="J9" s="169" t="s">
+      <c r="J9" s="190" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="177"/>
-      <c r="C10" s="177"/>
+      <c r="B10" s="179"/>
+      <c r="C10" s="179"/>
       <c r="D10" s="90" t="s">
         <v>182</v>
       </c>
@@ -14208,14 +14232,14 @@
       <c r="F10" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="180"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="191"/>
-      <c r="J10" s="170"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="185"/>
+      <c r="I10" s="196"/>
+      <c r="J10" s="191"/>
     </row>
     <row r="11" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="178"/>
-      <c r="C11" s="178"/>
+      <c r="B11" s="180"/>
+      <c r="C11" s="180"/>
       <c r="D11" s="93" t="s">
         <v>7</v>
       </c>
@@ -14225,16 +14249,16 @@
       <c r="F11" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="181"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="192"/>
-      <c r="J11" s="171"/>
+      <c r="G11" s="183"/>
+      <c r="H11" s="186"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="192"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="159" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="155" t="s">
+      <c r="C12" s="159" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="61" t="s">
@@ -14246,22 +14270,22 @@
       <c r="F12" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="G12" s="146" t="s">
+      <c r="G12" s="161" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="148" t="s">
+      <c r="H12" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="150" t="s">
+      <c r="I12" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="J12" s="164" t="s">
+      <c r="J12" s="155" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="156"/>
-      <c r="C13" s="156"/>
+      <c r="B13" s="169"/>
+      <c r="C13" s="169"/>
       <c r="D13" s="64" t="s">
         <v>182</v>
       </c>
@@ -14271,14 +14295,14 @@
       <c r="F13" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="G13" s="158"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="168"/>
+      <c r="G13" s="170"/>
+      <c r="H13" s="171"/>
+      <c r="I13" s="172"/>
+      <c r="J13" s="163"/>
     </row>
     <row r="14" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="156"/>
-      <c r="C14" s="156"/>
+      <c r="B14" s="169"/>
+      <c r="C14" s="169"/>
       <c r="D14" s="48" t="s">
         <v>7</v>
       </c>
@@ -14288,14 +14312,14 @@
       <c r="F14" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="G14" s="158"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="168"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="171"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="163"/>
     </row>
     <row r="15" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="157"/>
-      <c r="C15" s="157"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
       <c r="D15" s="67" t="s">
         <v>82</v>
       </c>
@@ -14305,10 +14329,10 @@
       <c r="F15" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="G15" s="147"/>
-      <c r="H15" s="149"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="165"/>
+      <c r="G15" s="162"/>
+      <c r="H15" s="152"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="156"/>
     </row>
     <row r="16" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
@@ -15997,11 +16021,18 @@
     <filterColumn colId="6" showButton="0"/>
   </autoFilter>
   <mergeCells count="29">
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
@@ -16014,18 +16045,11 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16050,29 +16074,29 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="132" t="s">
+      <c r="E2" s="138"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="130" t="s">
+      <c r="H2" s="138"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="135" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
@@ -16091,7 +16115,7 @@
       <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="131"/>
+      <c r="J3" s="136"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>

</xml_diff>